<commit_message>
feat: secuence reset Test data
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andreea.ghetu\Documents\UiPath\CSharpChanges\StudioTemplates\REFramework\C#\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPathPrograms\Performer_ContabilidadFacturas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96902286-4E3C-425E-A0BF-F83C72A8C5F4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4DD5FC-9481-4922-9E58-FE0A34B92254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18000" windowHeight="9480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="5550" windowWidth="16860" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -88,10 +88,6 @@
   </si>
   <si>
     <t>Framework</t>
-  </si>
-  <si>
-    <t>ProcessABCQueue</t>
-    <phoneticPr fontId="2"/>
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
@@ -161,6 +157,39 @@
   </si>
   <si>
     <t>Folder name. The value must match a folder defined in Orchestrator and queue specified as OrchestratorQueueName should be created in this folder. For classic folders leave the value field empty.</t>
+  </si>
+  <si>
+    <t>PathExceptionsFile</t>
+  </si>
+  <si>
+    <t>Data\\Exceptions.xlsx</t>
+  </si>
+  <si>
+    <t>PathLogs</t>
+  </si>
+  <si>
+    <t>C:\Vendors\Logs\</t>
+  </si>
+  <si>
+    <t>PathExcel</t>
+  </si>
+  <si>
+    <t>C:\Vendors\Vendor List.xlsx</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/home</t>
+  </si>
+  <si>
+    <t>Contabilidad_Facturas</t>
+  </si>
+  <si>
+    <t>URL_ResetData</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/reset-test-data</t>
   </si>
 </sst>
 </file>
@@ -212,21 +241,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -245,7 +270,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -541,13 +566,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z5"/>
+  <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
@@ -591,25 +616,25 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="7" t="s">
-        <v>38</v>
+      <c r="A3" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="7"/>
+      <c r="A4" s="2"/>
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
@@ -619,8 +644,51 @@
         <v>21</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>24</v>
-      </c>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
+      <c r="B12" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>
@@ -637,7 +705,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -687,24 +755,22 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="45">
-      <c r="A3" s="5" t="s">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="4" spans="1:26">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="6"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:26">
       <c r="A5" t="s">
@@ -725,7 +791,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26">
@@ -747,7 +813,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26">
@@ -758,7 +824,7 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -769,56 +835,51 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="5">
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15">
         <v>2</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
-      <c r="A15" s="5" t="s">
+      <c r="C15" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="5">
-        <v>2</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="17" spans="1:3" ht="45">
-      <c r="A17" s="5" t="s">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +896,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>
@@ -851,7 +912,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
feat: sequence get credentials from assets
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPathPrograms\Performer_ContabilidadFacturas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4DD5FC-9481-4922-9E58-FE0A34B92254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DDD2FC-7C36-4782-900D-C02EA8452EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="5550" windowWidth="16860" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -162,9 +162,6 @@
     <t>PathExceptionsFile</t>
   </si>
   <si>
-    <t>Data\\Exceptions.xlsx</t>
-  </si>
-  <si>
     <t>PathLogs</t>
   </si>
   <si>
@@ -190,6 +187,21 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/reset-test-data</t>
+  </si>
+  <si>
+    <t>URL_Invoices</t>
+  </si>
+  <si>
+    <t>https://acme-test.uipath.com/invoices/search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserCredential </t>
+  </si>
+  <si>
+    <t>UserCredential</t>
+  </si>
+  <si>
+    <t>C:\Exceptions.xlsx</t>
   </si>
 </sst>
 </file>
@@ -241,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -251,7 +263,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,13 +580,13 @@
   <dimension ref="A1:Z12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
-    <col min="2" max="2" width="43" customWidth="1"/>
+    <col min="2" max="2" width="51.85546875" customWidth="1"/>
     <col min="3" max="3" width="81.42578125" customWidth="1"/>
     <col min="4" max="26" width="8.7109375" customWidth="1"/>
   </cols>
@@ -619,7 +630,7 @@
         <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -649,10 +660,10 @@
     </row>
     <row r="6" spans="1:26">
       <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
         <v>50</v>
-      </c>
-      <c r="B6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:26">
@@ -660,35 +671,48 @@
         <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:26">
       <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" t="s">
         <v>46</v>
-      </c>
-      <c r="B8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:26">
       <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
         <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:26">
       <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
         <v>53</v>
       </c>
-      <c r="B10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:26">
+      <c r="A11" t="s">
         <v>54</v>
       </c>
+      <c r="B11" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="12" spans="1:26">
-      <c r="B12" s="2"/>
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
feat: sequences move_VendorListExcel, Obtain_data, Reset_test_data, Write_Data
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UiPathPrograms\Performer_ContabilidadFacturas\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DDD2FC-7C36-4782-900D-C02EA8452EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66A69044-B28F-4ABF-9296-1008AC32B95A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1185" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-15495" yWindow="1305" windowWidth="14100" windowHeight="15210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="73">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +202,48 @@
   </si>
   <si>
     <t>C:\Exceptions.xlsx</t>
+  </si>
+  <si>
+    <t>BECode_Credential</t>
+  </si>
+  <si>
+    <t>BE#001</t>
+  </si>
+  <si>
+    <t>Client_Email</t>
+  </si>
+  <si>
+    <t>sarashattra@gmail.com</t>
+  </si>
+  <si>
+    <t>BE#003</t>
+  </si>
+  <si>
+    <t>BECode_Amount</t>
+  </si>
+  <si>
+    <t>BECode_NoInvoices</t>
+  </si>
+  <si>
+    <t>BE#005</t>
+  </si>
+  <si>
+    <t>BECode_NoEURInvoices</t>
+  </si>
+  <si>
+    <t>BE#004</t>
+  </si>
+  <si>
+    <t>SECode_ResetTestData</t>
+  </si>
+  <si>
+    <t>SE#006</t>
+  </si>
+  <si>
+    <t>Path_Output_Vendors</t>
+  </si>
+  <si>
+    <t>C:\Output_Vendors</t>
   </si>
 </sst>
 </file>
@@ -281,7 +323,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -577,13 +619,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z12"/>
+  <dimension ref="A1:Z19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="43.5703125" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
@@ -714,6 +756,62 @@
         <v>57</v>
       </c>
     </row>
+    <row r="13" spans="1:26">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+      <c r="B14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
+      <c r="A15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
+      <c r="A16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B19" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -725,11 +823,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
@@ -787,7 +885,7 @@
         <v>31</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>32</v>
@@ -920,7 +1018,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
     <col min="2" max="2" width="30.140625" customWidth="1"/>

</xml_diff>